<commit_message>
Merged with main branch.
</commit_message>
<xml_diff>
--- a/FPGA/documentation/ddc multiplexer design info.xlsx
+++ b/FPGA/documentation/ddc multiplexer design info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xilinxdesigns\Saturn\FPGA\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA975508-724D-4E97-BF71-497D772DE70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B2A0E4-7BE4-46AA-8818-1CAD70E9F23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8070" yWindow="3885" windowWidth="28800" windowHeight="15345" xr2:uid="{428FD10C-5BF3-4DAF-8DB8-B3D5A3135663}"/>
+    <workbookView xWindow="420" yWindow="2640" windowWidth="19980" windowHeight="17190" xr2:uid="{428FD10C-5BF3-4DAF-8DB8-B3D5A3135663}"/>
   </bookViews>
   <sheets>
     <sheet name="DDC data stream" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>DDC</t>
   </si>
@@ -87,13 +87,19 @@
   </si>
   <si>
     <t>DDC7</t>
+  </si>
+  <si>
+    <t>00001BF002FD11DA</t>
+  </si>
+  <si>
+    <t>000082E6E828F7EE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +111,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,15 +195,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -209,9 +221,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -249,7 +261,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -355,7 +367,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -497,7 +509,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -507,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24AA51B-5530-492B-8EAE-16B25F3F7DD0}">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:C46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,50 +569,50 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <f t="shared" ref="C2:K2" si="0">D2*8</f>
-        <v>134217728</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6">
+        <f>C2*8</f>
+        <v>8</v>
+      </c>
+      <c r="E2" s="6">
+        <f t="shared" ref="E2:L2" si="0">D2*8</f>
+        <v>64</v>
+      </c>
+      <c r="F2" s="6">
+        <f t="shared" si="0"/>
+        <v>512</v>
+      </c>
+      <c r="G2" s="6">
+        <f t="shared" si="0"/>
+        <v>4096</v>
+      </c>
+      <c r="H2" s="6">
+        <f t="shared" si="0"/>
+        <v>32768</v>
+      </c>
+      <c r="I2" s="6">
+        <f t="shared" si="0"/>
+        <v>262144</v>
+      </c>
+      <c r="J2" s="6">
+        <f t="shared" si="0"/>
+        <v>2097152</v>
+      </c>
+      <c r="K2" s="6">
         <f t="shared" si="0"/>
         <v>16777216</v>
       </c>
-      <c r="E2">
+      <c r="L2" s="6">
         <f t="shared" si="0"/>
-        <v>2097152</v>
-      </c>
-      <c r="F2">
-        <f t="shared" si="0"/>
-        <v>262144</v>
-      </c>
-      <c r="G2">
-        <f t="shared" si="0"/>
-        <v>32768</v>
-      </c>
-      <c r="H2">
-        <f t="shared" si="0"/>
-        <v>4096</v>
-      </c>
-      <c r="I2">
-        <f t="shared" si="0"/>
-        <v>512</v>
-      </c>
-      <c r="J2">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="K2">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
+        <v>134217728</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -630,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -665,7 +677,7 @@
         <v>48</v>
       </c>
       <c r="J4">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="K4">
         <v>48</v>
@@ -691,40 +703,34 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:L5" si="1">IF(G3=1,(G4/48)-1,7)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <f>C2*C5+D2*D5+E2*E5+F2*F5+G2*G5+H2*H5+I2*I5+J2*J5+K2*K5+L2*L5</f>
-        <v>461635583</v>
+        <v>4195099</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -732,8 +738,8 @@
         <v>6</v>
       </c>
       <c r="C7" t="str">
-        <f>_xlfn.CONCAT("10000000",DEC2HEX(C6,8))</f>
-        <v>100000001B83FFFF</v>
+        <f>_xlfn.CONCAT("80000000",DEC2HEX(C6,8))</f>
+        <v>800000000040031B</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -745,23 +751,23 @@
       </c>
       <c r="C8" t="str">
         <f ca="1">_xlfn.CONCAT(DEC2HEX(INT(RAND()*2^24),6), DEC2HEX(INT(RAND()*2^24),6))</f>
-        <v>EFB8165E22E9</v>
+        <v>C8563C6F857E</v>
       </c>
       <c r="D8" t="str">
         <f ca="1">_xlfn.CONCAT(DEC2HEX(INT(RAND()*2^24),6), DEC2HEX(INT(RAND()*2^24),6))</f>
-        <v>1ED999A9B06C</v>
+        <v>1CAAB89FACED</v>
       </c>
       <c r="E8" t="str">
         <f ca="1">_xlfn.CONCAT(DEC2HEX(INT(RAND()*2^24),6), DEC2HEX(INT(RAND()*2^24),6))</f>
-        <v>6C9AB7EC5211</v>
+        <v>676EE6B2E6B1</v>
       </c>
       <c r="F8" t="str">
         <f ca="1">_xlfn.CONCAT(DEC2HEX(INT(RAND()*2^24),6), DEC2HEX(INT(RAND()*2^24),6))</f>
-        <v>AC6D0D9E2627</v>
+        <v>0BFC5E0B4B52</v>
       </c>
       <c r="J8" t="str">
         <f ca="1">_xlfn.CONCAT(DEC2HEX(INT(RAND()*2^24),6), DEC2HEX(INT(RAND()*2^24),6))</f>
-        <v>6878189F1D42</v>
+        <v>F5DCD9E58102</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -769,20 +775,20 @@
         <v>1</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" ref="C9:E15" ca="1" si="2">_xlfn.CONCAT(DEC2HEX(INT(RAND()*2^24),6), DEC2HEX(INT(RAND()*2^24),6))</f>
-        <v>E2CC5C33D1A2</v>
+        <f t="shared" ref="C9:E15" ca="1" si="1">_xlfn.CONCAT(DEC2HEX(INT(RAND()*2^24),6), DEC2HEX(INT(RAND()*2^24),6))</f>
+        <v>2CED82010471</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>7C83BB2AF529</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6232B93FE683</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>0339A05855F7</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5F3E3E5CA838</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" ref="J9" ca="1" si="3">_xlfn.CONCAT(DEC2HEX(INT(RAND()*2^24),6), DEC2HEX(INT(RAND()*2^24),6))</f>
-        <v>2A6C332867B2</v>
+        <f t="shared" ref="J9" ca="1" si="2">_xlfn.CONCAT(DEC2HEX(INT(RAND()*2^24),6), DEC2HEX(INT(RAND()*2^24),6))</f>
+        <v>2A06AF93E9D4</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -790,16 +796,16 @@
         <v>2</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>26BB315B49EA</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4BA8511A2051</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>288B1E95D38D</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6857D97CD621</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>B5444920AF82</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>D9AA00B3C89C</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -807,16 +813,16 @@
         <v>3</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>5148B9A13644</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2307BBFD2533</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>8919B9CCEF73</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5981BC098A7B</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>F3F9C2FE4E14</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2031548CEFD3</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -825,7 +831,7 @@
       </c>
       <c r="E12" t="str">
         <f ca="1">_xlfn.CONCAT(DEC2HEX(INT(RAND()*2^24),6), DEC2HEX(INT(RAND()*2^24),6))</f>
-        <v>B7D4BF1EEBA4</v>
+        <v>59685143568C</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -833,8 +839,8 @@
         <v>5</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>924C9D9162C3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>218B1F1AA5FC</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -842,8 +848,8 @@
         <v>6</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>6BE5A771F08F</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1AD6F77D460F</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -851,8 +857,8 @@
         <v>7</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>F4189ECCBE4A</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>124911BDEE1C</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -863,24 +869,24 @@
         <v>9</v>
       </c>
       <c r="C16" t="str">
-        <f ca="1">_xlfn.CONCAT(DEC2HEX(((C$1*256)+$A16),4),C8)</f>
-        <v>0000EFB8165E22E9</v>
+        <f ca="1">_xlfn.CONCAT(DEC2HEX(0,4),C8)</f>
+        <v>0000C8563C6F857E</v>
       </c>
       <c r="D16" t="str">
-        <f ca="1">_xlfn.CONCAT(DEC2HEX(((D$1*256)+$A16),4),D8)</f>
-        <v>01001ED999A9B06C</v>
+        <f ca="1">_xlfn.CONCAT(DEC2HEX(0,4),D8)</f>
+        <v>00001CAAB89FACED</v>
       </c>
       <c r="E16" t="str">
-        <f ca="1">_xlfn.CONCAT(DEC2HEX(((E$1*256)+$A16),4),E8)</f>
-        <v>02006C9AB7EC5211</v>
+        <f ca="1">_xlfn.CONCAT(DEC2HEX(0,4),E8)</f>
+        <v>0000676EE6B2E6B1</v>
       </c>
       <c r="F16" t="str">
-        <f ca="1">_xlfn.CONCAT(DEC2HEX(((F$1*256)+$A16),4),F8)</f>
-        <v>0300AC6D0D9E2627</v>
+        <f ca="1">_xlfn.CONCAT(DEC2HEX(0,4),F8)</f>
+        <v>00000BFC5E0B4B52</v>
       </c>
       <c r="J16" t="str">
-        <f ca="1">_xlfn.CONCAT(DEC2HEX(((J$1*256)+$A16),4),J8)</f>
-        <v>07006878189F1D42</v>
+        <f ca="1">_xlfn.CONCAT(DEC2HEX(0,4),J8)</f>
+        <v>0000F5DCD9E58102</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -888,20 +894,20 @@
         <v>1</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" ref="C17:D19" ca="1" si="4">_xlfn.CONCAT(DEC2HEX(((C$1*256)+$A17),4),C9)</f>
-        <v>0001E2CC5C33D1A2</v>
+        <f t="shared" ref="C17:D23" ca="1" si="3">_xlfn.CONCAT(DEC2HEX(0,4),C9)</f>
+        <v>00002CED82010471</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>01017C83BB2AF529</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>00006232B93FE683</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" ref="E17" ca="1" si="5">_xlfn.CONCAT(DEC2HEX(((E$1*256)+$A17),4),E9)</f>
-        <v>02010339A05855F7</v>
+        <f t="shared" ref="E17" ca="1" si="4">_xlfn.CONCAT(DEC2HEX(0,4),E9)</f>
+        <v>00005F3E3E5CA838</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" ref="J17" ca="1" si="6">_xlfn.CONCAT(DEC2HEX(((J$1*256)+$A17),4),J9)</f>
-        <v>07012A6C332867B2</v>
+        <f t="shared" ref="J17" ca="1" si="5">_xlfn.CONCAT(DEC2HEX(0,4),J9)</f>
+        <v>00002A06AF93E9D4</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -909,16 +915,16 @@
         <v>2</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>000226BB315B49EA</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>00004BA8511A2051</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>0102288B1E95D38D</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>00006857D97CD621</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" ref="E18" ca="1" si="7">_xlfn.CONCAT(DEC2HEX(((E$1*256)+$A18),4),E10)</f>
-        <v>0202B5444920AF82</v>
+        <f t="shared" ref="E18" ca="1" si="6">_xlfn.CONCAT(DEC2HEX(0,4),E10)</f>
+        <v>0000D9AA00B3C89C</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -926,16 +932,16 @@
         <v>3</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>00035148B9A13644</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>00002307BBFD2533</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>01038919B9CCEF73</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>00005981BC098A7B</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" ref="E19" ca="1" si="8">_xlfn.CONCAT(DEC2HEX(((E$1*256)+$A19),4),E11)</f>
-        <v>0203F3F9C2FE4E14</v>
+        <f t="shared" ref="E19" ca="1" si="7">_xlfn.CONCAT(DEC2HEX(0,4),E11)</f>
+        <v>00002031548CEFD3</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -943,8 +949,8 @@
         <v>4</v>
       </c>
       <c r="E20" t="str">
-        <f ca="1">_xlfn.CONCAT(DEC2HEX(((E$1*256)+$A20),4),E12)</f>
-        <v>0204B7D4BF1EEBA4</v>
+        <f ca="1">_xlfn.CONCAT(DEC2HEX(0,4),E12)</f>
+        <v>000059685143568C</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -952,8 +958,8 @@
         <v>5</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" ref="E21" ca="1" si="9">_xlfn.CONCAT(DEC2HEX(((E$1*256)+$A21),4),E13)</f>
-        <v>0205924C9D9162C3</v>
+        <f t="shared" ref="E21:E23" ca="1" si="8">_xlfn.CONCAT(DEC2HEX(0,4),E13)</f>
+        <v>0000218B1F1AA5FC</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -961,8 +967,8 @@
         <v>6</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" ref="E22" ca="1" si="10">_xlfn.CONCAT(DEC2HEX(((E$1*256)+$A22),4),E14)</f>
-        <v>02066BE5A771F08F</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>00001AD6F77D460F</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -970,8 +976,8 @@
         <v>7</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" ref="E23" ca="1" si="11">_xlfn.CONCAT(DEC2HEX(((E$1*256)+$A23),4),E15)</f>
-        <v>0207F4189ECCBE4A</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0000124911BDEE1C</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -982,7 +988,7 @@
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="str">
         <f>C7</f>
-        <v>100000001B83FFFF</v>
+        <v>800000000040031B</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
@@ -991,7 +997,7 @@
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="str">
         <f ca="1">C16</f>
-        <v>0000EFB8165E22E9</v>
+        <v>0000C8563C6F857E</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
@@ -999,26 +1005,26 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="str">
-        <f t="shared" ref="B29:B31" ca="1" si="12">C17</f>
-        <v>0001E2CC5C33D1A2</v>
+        <f t="shared" ref="B29:B31" ca="1" si="9">C17</f>
+        <v>00002CED82010471</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>000226BB315B49EA</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>00004BA8511A2051</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>00035148B9A13644</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>00002307BBFD2533</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="str">
         <f ca="1">D16</f>
-        <v>01001ED999A9B06C</v>
+        <v>00001CAAB89FACED</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
@@ -1026,26 +1032,26 @@
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="str">
-        <f t="shared" ref="B33:B35" ca="1" si="13">D17</f>
-        <v>01017C83BB2AF529</v>
+        <f t="shared" ref="B33:B35" ca="1" si="10">D17</f>
+        <v>00006232B93FE683</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v>0102288B1E95D38D</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>00006857D97CD621</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v>01038919B9CCEF73</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>00005981BC098A7B</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="str">
         <f ca="1">E16</f>
-        <v>02006C9AB7EC5211</v>
+        <v>0000676EE6B2E6B1</v>
       </c>
       <c r="C36" t="s">
         <v>13</v>
@@ -1053,68 +1059,68 @@
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="str">
-        <f t="shared" ref="B37:B43" ca="1" si="14">E17</f>
-        <v>02010339A05855F7</v>
+        <f t="shared" ref="B37:B43" ca="1" si="11">E17</f>
+        <v>00005F3E3E5CA838</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v>0202B5444920AF82</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0000D9AA00B3C89C</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v>0203F3F9C2FE4E14</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>00002031548CEFD3</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v>0204B7D4BF1EEBA4</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>000059685143568C</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v>0205924C9D9162C3</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0000218B1F1AA5FC</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v>02066BE5A771F08F</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>00001AD6F77D460F</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v>0207F4189ECCBE4A</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0000124911BDEE1C</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="str">
         <f ca="1">F16</f>
-        <v>0300AC6D0D9E2627</v>
+        <v>00000BFC5E0B4B52</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="6" t="str">
+      <c r="B45" s="2" t="str">
         <f ca="1">J16</f>
-        <v>07006878189F1D42</v>
+        <v>0000F5DCD9E58102</v>
       </c>
       <c r="C45" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="7" t="str">
+      <c r="B46" s="4" t="str">
         <f ca="1">J17</f>
-        <v>07012A6C332867B2</v>
+        <v>00002A06AF93E9D4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>